<commit_message>
Updated U5 population size
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -3115,8 +3115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3137,7 +3137,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="18">
-        <v>9419084</v>
+        <v>9622975</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6308,7 +6308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated spreadsheets to those containing new IYCF1.0
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/2017Sep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jankapetravic/Documents/OPTIMA/Optima nutrition/Tanzania/Input sheets/input v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="7100" yWindow="2660" windowWidth="19500" windowHeight="21940" tabRatio="500" firstSheet="18" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -1133,7 +1133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="86">
   <si>
     <t>indicators</t>
   </si>
@@ -1376,6 +1376,21 @@
   </si>
   <si>
     <t>Vitamin A fortification of food</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food secure with IYCF)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food secure without IYCF)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food insecure with IYCF and supplementation)</t>
+  </si>
+  <si>
+    <t>Complementary feeding (food insecure with neither IYCF nor supplementation)</t>
+  </si>
+  <si>
+    <t>IYCF</t>
   </si>
 </sst>
 </file>
@@ -1467,7 +1482,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1510,6 +1525,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1520,7 +1541,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1578,8 +1599,128 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1640,8 +1781,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="177">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1670,6 +1812,66 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1697,6 +1899,66 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -3115,7 +3377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -4444,10 +4706,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A7" sqref="A7:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4555,6 +4817,86 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1.43</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1.43</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
+        <v>2.39</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2.39</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4565,7 +4907,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4634,13 +4976,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="12">
+        <v>5.16</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5.16</v>
+      </c>
+      <c r="D4" s="12">
+        <v>1.82</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1.82</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4854,8 +5208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4997,6 +5351,18 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="C9" s="32">
+        <v>0.95</v>
+      </c>
+      <c r="D9" s="24">
+        <v>10.49</v>
+      </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>

</xml_diff>

<commit_message>
modified national spreadsheet to replace BF and CFE with IYCF
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jankapetravic/Documents/OPTIMA/Optima nutrition/Tanzania/Input sheets/input v2/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7100" yWindow="2660" windowWidth="19500" windowHeight="21940" tabRatio="500" firstSheet="18" activeTab="19"/>
+    <workbookView xWindow="1900" yWindow="460" windowWidth="20960" windowHeight="12480" tabRatio="500" firstSheet="19" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -38,13 +33,13 @@
     <sheet name="Interventions mortality eff" sheetId="24" r:id="rId24"/>
     <sheet name="Interventions incidence eff" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -811,6 +806,28 @@
         </r>
       </text>
     </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Bangladesh cost</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D4" authorId="0">
       <text>
         <r>
@@ -830,76 +847,54 @@
           </rPr>
           <t xml:space="preserve">
 Bangladesh cost</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+IFAS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Cochrane review - not finished; no who guidelines.</t>
         </r>
       </text>
     </comment>
     <comment ref="D6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Bangladesh cost</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-IFAS</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Cochrane review - not finished; no who guidelines.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -932,7 +927,7 @@
     <author xml:space="preserve"> Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0">
+    <comment ref="D3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -954,7 +949,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="E3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -976,7 +971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0">
+    <comment ref="G4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -998,7 +993,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="1">
+    <comment ref="A5" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1133,7 +1128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="80">
   <si>
     <t>indicators</t>
   </si>
@@ -1357,12 +1352,6 @@
     <t>Prophylactic zinc supplementation</t>
   </si>
   <si>
-    <t>Breastfeeding promotion</t>
-  </si>
-  <si>
-    <t>Complementary feeding education</t>
-  </si>
-  <si>
     <t>Public provision of complementary foods</t>
   </si>
   <si>
@@ -1376,18 +1365,6 @@
   </si>
   <si>
     <t>Vitamin A fortification of food</t>
-  </si>
-  <si>
-    <t>Complementary feeding (food secure with IYCF)</t>
-  </si>
-  <si>
-    <t>Complementary feeding (food secure without IYCF)</t>
-  </si>
-  <si>
-    <t>Complementary feeding (food insecure with IYCF and supplementation)</t>
-  </si>
-  <si>
-    <t>Complementary feeding (food insecure with neither IYCF nor supplementation)</t>
   </si>
   <si>
     <t>IYCF</t>
@@ -3377,16 +3354,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+    <sheetView zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3394,7 +3371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -3402,7 +3379,7 @@
         <v>9622975</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
@@ -3410,7 +3387,7 @@
         <v>2070000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -3418,7 +3395,7 @@
         <v>2433877.8870553677</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>71</v>
       </c>
@@ -3426,7 +3403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>70</v>
       </c>
@@ -3434,7 +3411,7 @@
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>72</v>
       </c>
@@ -3446,6 +3423,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3457,12 +3439,12 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -3485,7 +3467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3508,7 +3490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
@@ -3528,7 +3510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>47</v>
       </c>
@@ -3548,7 +3530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>48</v>
       </c>
@@ -3568,7 +3550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -3591,7 +3573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
@@ -3611,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>47</v>
       </c>
@@ -3631,7 +3613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>48</v>
       </c>
@@ -3651,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3674,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -3694,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -3714,7 +3696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -3734,7 +3716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -3757,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
@@ -3777,7 +3759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>47</v>
       </c>
@@ -3797,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
@@ -3817,7 +3799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -3840,7 +3822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
@@ -3860,7 +3842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>47</v>
       </c>
@@ -3880,7 +3862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>48</v>
       </c>
@@ -3900,7 +3882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="15.75" customHeight="1">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3923,7 +3905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="15.75" customHeight="1">
       <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
@@ -3943,7 +3925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="15.75" customHeight="1">
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
@@ -3963,7 +3945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="15.75" customHeight="1">
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
@@ -3983,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="15.75" customHeight="1">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -4006,7 +3988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="15.75" customHeight="1">
       <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
@@ -4026,7 +4008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" ht="15.75" customHeight="1">
       <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
@@ -4046,7 +4028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" ht="15.75" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>48</v>
       </c>
@@ -4068,6 +4050,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4079,13 +4066,13 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -4102,7 +4089,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
@@ -4121,7 +4108,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="s">
         <v>21</v>
       </c>
@@ -4140,7 +4127,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>22</v>
       </c>
@@ -4159,7 +4146,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -4178,7 +4165,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
@@ -4197,7 +4184,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
@@ -4216,7 +4203,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
         <v>54</v>
       </c>
@@ -4235,7 +4222,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>31</v>
       </c>
@@ -4254,113 +4241,118 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:7" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:7" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:7" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:7" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:7" ht="15.75" customHeight="1">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:7" ht="15.75" customHeight="1">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:7" ht="15.75" customHeight="1">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:7" ht="15.75" customHeight="1">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:7" ht="15.75" customHeight="1">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:7" ht="15.75" customHeight="1">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:7" ht="15.75" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4372,9 +4364,9 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -4388,7 +4380,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="5">
         <v>45</v>
       </c>
@@ -4404,6 +4396,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4413,12 +4410,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>55</v>
       </c>
@@ -4438,7 +4435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>45</v>
       </c>
@@ -4458,7 +4455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
@@ -4478,7 +4475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
@@ -4498,7 +4495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
@@ -4520,6 +4517,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4531,9 +4533,9 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -4553,7 +4555,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -4575,6 +4577,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4586,9 +4593,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
@@ -4602,7 +4609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -4618,6 +4625,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4629,12 +4641,12 @@
       <selection activeCell="E30" sqref="E29:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4654,7 +4666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>73</v>
       </c>
@@ -4674,7 +4686,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -4682,7 +4694,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -4690,7 +4702,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -4701,25 +4713,30 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="70.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -4737,7 +4754,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>57</v>
       </c>
@@ -4757,7 +4774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
@@ -4777,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -4797,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
@@ -4817,106 +4834,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1.43</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1.43</v>
-      </c>
-      <c r="F8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
-        <v>2.39</v>
-      </c>
-      <c r="E10" s="5">
-        <v>2.39</v>
-      </c>
-      <c r="F10" s="5">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:F4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -4936,9 +4878,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B2" s="12">
         <v>5.16</v>
@@ -4947,57 +4889,22 @@
         <v>5.16</v>
       </c>
       <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="13">
-        <v>1</v>
+        <v>1.82</v>
+      </c>
+      <c r="E2" s="14">
+        <v>1.82</v>
       </c>
       <c r="F2" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12">
-        <v>1</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1.82</v>
-      </c>
-      <c r="E3" s="14">
-        <v>1.82</v>
-      </c>
-      <c r="F3" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="12">
-        <v>5.16</v>
-      </c>
-      <c r="C4" s="12">
-        <v>5.16</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1.82</v>
-      </c>
-      <c r="E4" s="14">
-        <v>1.82</v>
-      </c>
-      <c r="F4" s="14">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5007,12 +4914,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -5029,7 +4936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="14">
       <c r="A2" s="12" t="s">
         <v>45</v>
       </c>
@@ -5046,14 +4953,14 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -5062,6 +4969,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5073,13 +4985,13 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -5087,7 +4999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>2017</v>
       </c>
@@ -5095,7 +5007,7 @@
         <v>2110000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="4">
         <v>2018</v>
       </c>
@@ -5103,7 +5015,7 @@
         <v>2150000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="4">
         <v>2019</v>
       </c>
@@ -5111,7 +5023,7 @@
         <v>2200000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
       <c r="A5" s="4">
         <v>2020</v>
       </c>
@@ -5119,7 +5031,7 @@
         <v>2240000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="4">
         <v>2021</v>
       </c>
@@ -5127,7 +5039,7 @@
         <v>2280000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="4">
         <v>2022</v>
       </c>
@@ -5135,7 +5047,7 @@
         <v>2330000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="4">
         <v>2023</v>
       </c>
@@ -5143,7 +5055,7 @@
         <v>2380000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="4">
         <v>2024</v>
       </c>
@@ -5151,7 +5063,7 @@
         <v>2420000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="4">
         <v>2025</v>
       </c>
@@ -5159,7 +5071,7 @@
         <v>2480000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="4">
         <v>2026</v>
       </c>
@@ -5167,7 +5079,7 @@
         <v>2530000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="4">
         <v>2027</v>
       </c>
@@ -5175,7 +5087,7 @@
         <v>2580000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="4">
         <v>2028</v>
       </c>
@@ -5183,7 +5095,7 @@
         <v>2630000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>2029</v>
       </c>
@@ -5191,7 +5103,7 @@
         <v>2690000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="4">
         <v>2030</v>
       </c>
@@ -5201,18 +5113,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.83203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -5220,7 +5137,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -5234,7 +5151,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5251,26 +5168,26 @@
       <c r="F2" s="15"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="24">
-        <v>0.19939999999999999</v>
-      </c>
-      <c r="C3" s="24">
+        <v>74</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
         <v>0.95</v>
       </c>
-      <c r="D3" s="24">
-        <v>11.19</v>
+      <c r="D3" s="25">
+        <v>48</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="15"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>76</v>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>75</v>
       </c>
       <c r="B4" s="5">
         <v>0</v>
@@ -5279,179 +5196,150 @@
         <v>0.95</v>
       </c>
       <c r="D4" s="25">
-        <v>48</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>74</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>77</v>
       </c>
       <c r="B5" s="24">
-        <v>0.23080000000000001</v>
+        <v>0.3538</v>
       </c>
       <c r="C5" s="24">
         <v>0.95</v>
       </c>
       <c r="D5" s="24">
-        <v>26.05</v>
+        <v>3.42</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="15"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="24">
+        <v>0</v>
+      </c>
+      <c r="C6" s="26">
         <v>0.95</v>
       </c>
-      <c r="D6" s="25">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+      <c r="D6" s="24">
+        <v>0.32</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="24">
-        <v>0.3538</v>
-      </c>
-      <c r="C7" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="32">
         <v>0.95</v>
       </c>
       <c r="D7" s="24">
-        <v>3.42</v>
+        <v>10.49</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="24">
-        <v>0</v>
-      </c>
-      <c r="C8" s="26">
-        <v>0.95</v>
-      </c>
-      <c r="D8" s="24">
-        <v>0.32</v>
-      </c>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B8" s="5"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="24">
-        <v>0.15</v>
-      </c>
-      <c r="C9" s="32">
-        <v>0.95</v>
-      </c>
-      <c r="D9" s="24">
-        <v>10.49</v>
-      </c>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="B9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" ht="15.75" customHeight="1">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="6" width="13.5" customWidth="1"/>
@@ -5461,7 +5349,7 @@
     <col min="10" max="10" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -5486,7 +5374,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5509,9 +5397,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -5520,105 +5408,105 @@
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
         <f>demographics!$B$6</f>
         <v>0.28199999999999997</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E3" s="4">
         <f>demographics!$B$6</f>
         <v>0.28199999999999997</v>
       </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
       <c r="F4" s="4">
         <v>0</v>
       </c>
       <c r="G4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
         <f>demographics!$B$6</f>
         <v>0.28199999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -5627,102 +5515,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+      <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="B10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="B11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" ht="15.75" customHeight="1">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" ht="15.75" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" ht="15.75" customHeight="1">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" ht="15.75" customHeight="1">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" ht="15.75" customHeight="1">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5734,12 +5598,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
@@ -5759,9 +5623,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>66</v>
@@ -5779,16 +5643,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="B3" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="16">
-        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
+        <f>demographics!$B$5 * 'Interventions target population'!$G$4</f>
         <v>0.28199999999999997</v>
       </c>
       <c r="D3" s="16">
-        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
+        <f>demographics!$B$5 * 'Interventions target population'!$G$4</f>
         <v>0.28199999999999997</v>
       </c>
       <c r="E3" s="16">
@@ -5798,9 +5662,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>66</v>
@@ -5818,7 +5682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="B5" t="s">
         <v>69</v>
       </c>
@@ -5835,14 +5699,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -5852,6 +5716,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5863,12 +5732,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -5891,7 +5760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -5914,7 +5783,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -5934,9 +5803,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>34</v>
@@ -5957,7 +5826,7 @@
         <v>0.41599999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -5981,6 +5850,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5992,12 +5866,12 @@
       <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -6020,7 +5894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -6043,7 +5917,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -6063,9 +5937,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>34</v>
@@ -6089,7 +5963,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -6113,6 +5987,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6124,12 +6003,12 @@
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>68</v>
       </c>
@@ -6152,7 +6031,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>64</v>
       </c>
@@ -6175,7 +6054,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
@@ -6195,9 +6074,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>34</v>
@@ -6221,7 +6100,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>36</v>
       </c>
@@ -6245,6 +6124,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6256,9 +6140,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -6269,7 +6153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="6">
         <v>25</v>
       </c>
@@ -6284,6 +6168,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6295,12 +6184,12 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -6320,7 +6209,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6340,7 +6229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -6360,7 +6249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -6380,7 +6269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -6400,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -6420,7 +6309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -6440,7 +6329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -6460,7 +6349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -6480,7 +6369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -6500,7 +6389,7 @@
         <v>0.1368</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -6520,7 +6409,7 @@
         <v>0.20660000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -6540,7 +6429,7 @@
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -6560,7 +6449,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -6580,7 +6469,7 @@
         <v>8.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -6600,7 +6489,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -6620,7 +6509,7 @@
         <v>1.5299999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -6640,7 +6529,7 @@
         <v>0.13589999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -6667,6 +6556,11 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="8" max="1048575" man="1"/>
   </colBreaks>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6678,9 +6572,9 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
@@ -6703,7 +6597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -6731,7 +6625,7 @@
         <v>23.259986385548594</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -6756,7 +6650,7 @@
         <v>37.370013614451409</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -6776,7 +6670,7 @@
         <v>25.94</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -6796,7 +6690,7 @@
         <v>13.43</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
@@ -6819,7 +6713,7 @@
         <v>48.515000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -6839,7 +6733,7 @@
         <v>48.515000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -6859,7 +6753,7 @@
         <v>2.2399999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -6879,7 +6773,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -6902,7 +6796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>46</v>
       </c>
@@ -6922,7 +6816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
@@ -6942,7 +6836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>48</v>
       </c>
@@ -6967,6 +6861,11 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6978,9 +6877,9 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
@@ -6991,7 +6890,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="7">
         <v>1.84E-2</v>
       </c>
@@ -7004,6 +6903,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7015,9 +6919,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -7037,7 +6941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -7057,7 +6961,7 @@
         <v>2.041525424</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
@@ -7081,6 +6985,11 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7090,9 +6999,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -7115,7 +7024,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -7138,7 +7047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -7158,7 +7067,7 @@
         <v>1.67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -7178,7 +7087,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -7198,7 +7107,7 @@
         <v>6.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -7221,7 +7130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -7241,7 +7150,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -7261,7 +7170,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -7281,7 +7190,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -7304,7 +7213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -7324,7 +7233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -7344,7 +7253,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -7364,7 +7273,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -7387,7 +7296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -7407,7 +7316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -7427,7 +7336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -7447,7 +7356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -7470,7 +7379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -7490,7 +7399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -7510,7 +7419,7 @@
         <v>1.86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -7532,6 +7441,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7541,9 +7455,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -7566,7 +7480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -7589,7 +7503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
@@ -7609,7 +7523,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>32</v>
       </c>
@@ -7629,7 +7543,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
@@ -7649,7 +7563,7 @@
         <v>12.33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -7672,7 +7586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
@@ -7692,7 +7606,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>32</v>
       </c>
@@ -7712,7 +7626,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
@@ -7732,7 +7646,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -7755,7 +7669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -7775,7 +7689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
@@ -7795,7 +7709,7 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
@@ -7815,7 +7729,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -7838,7 +7752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>29</v>
       </c>
@@ -7858,7 +7772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
@@ -7878,7 +7792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="B17" s="5" t="s">
         <v>33</v>
       </c>
@@ -7898,7 +7812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -7921,7 +7835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -7941,7 +7855,7 @@
         <v>1.65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="15.75" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>32</v>
       </c>
@@ -7961,7 +7875,7 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="15.75" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
@@ -7983,5 +7897,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed baseline coverage of IYCF to 0 from 0.15
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
+++ b/input_spreadsheets/Tanzania/2017Sep/InputForCode_Tanzania.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="460" windowWidth="20960" windowHeight="12480" tabRatio="500" firstSheet="19" activeTab="20"/>
+    <workbookView xWindow="1900" yWindow="460" windowWidth="20960" windowHeight="12480" tabRatio="500" firstSheet="19" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -5125,8 +5125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -5238,7 +5238,7 @@
         <v>79</v>
       </c>
       <c r="B7" s="24">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="C7" s="32">
         <v>0.95</v>
@@ -5335,7 +5335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>